<commit_message>
Week 2 and 3
</commit_message>
<xml_diff>
--- a/gradesheet.xlsx
+++ b/gradesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PPL-CSCI-3155\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50982844-FD56-4805-8D72-B33BE81B52C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AA8A59-5C3B-4E36-B8F4-862AD4DE6FC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9900" windowWidth="29040" windowHeight="15840" xr2:uid="{A5203DAB-6FA8-4205-80AF-4B5C077A9E25}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Spot Exams</t>
-  </si>
-  <si>
-    <t>Problem Sets</t>
   </si>
   <si>
     <t>Mini Projects</t>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Assignments</t>
   </si>
 </sst>
 </file>
@@ -139,48 +139,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color auto="1"/>
@@ -213,91 +172,12 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
         <color auto="1"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -328,656 +208,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF009900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1300,29 +530,30 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
     <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1342,8 +573,12 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="1">
+        <v>100</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1405,11 +640,11 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2" t="e">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1429,16 +664,16 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="e">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2">
         <f>AVERAGE(C:C)</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L6" s="4" t="e">
         <f>((0.1 * H5) + (0.3 * H6) + (0.1 * H7) + (0.3 * H8))/0.8</f>
@@ -1458,7 +693,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="2" t="e">
         <f>AVERAGE(D:D)</f>
@@ -1467,7 +702,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L7" s="4" t="e">
         <f>(0.1 * H5) + (0.3 * H6) + (0.1 * H7) + (0.3 * H8) + (0.2 * H9)</f>
@@ -1487,7 +722,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="2" t="e">
         <f>AVERAGE(E:E)</f>
@@ -1511,10 +746,10 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1677,7 +912,9 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1882,13 +1119,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>70</formula>
       <formula>79.9999</formula>
     </cfRule>
@@ -1897,13 +1134,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:L7">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThanOrEqual">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
       <formula>70</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
       <formula>70</formula>
       <formula>79.9999</formula>
     </cfRule>

</xml_diff>